<commit_message>
ideas to record and scenario
</commit_message>
<xml_diff>
--- a/resources/Brain Dump.xlsx
+++ b/resources/Brain Dump.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkork\OneDrive\Desktop\EDTH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\echologia\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9F58CC6-6511-47B1-AE46-21CCFED46B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53A452CA-3E4F-43F8-A9D4-65F791286123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C544BCDC-9C78-46B8-B4C5-15391AB69DE9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Attributes for detection" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>open source librayr</t>
   </si>
@@ -87,13 +88,259 @@
   </si>
   <si>
     <t>Recongnize</t>
+  </si>
+  <si>
+    <t>data basesfor raw data</t>
+  </si>
+  <si>
+    <t>list of files</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>What It Reveals</t>
+  </si>
+  <si>
+    <t>Typical Sound Cues / Tags</t>
+  </si>
+  <si>
+    <t>Detection Module(s)</t>
+  </si>
+  <si>
+    <t>Dataset(s) / Source</t>
+  </si>
+  <si>
+    <t>Geolocation / Scene Type</t>
+  </si>
+  <si>
+    <t>Traffic hum, horns, church bells, seagulls, waves, wind in trees, HVAC, metro sounds</t>
+  </si>
+  <si>
+    <t>PANNs / YAMNet / EfficientAT</t>
+  </si>
+  <si>
+    <t>DCASE (Acoustic Scene), FSD50K</t>
+  </si>
+  <si>
+    <t>Mobility / Transport Mode</t>
+  </si>
+  <si>
+    <t>Type of vehicle, movement, terrain</t>
+  </si>
+  <si>
+    <t>YAMNet, CLAP query (“rotor noise”)</t>
+  </si>
+  <si>
+    <t>AudioSet, AeroSonicDB</t>
+  </si>
+  <si>
+    <t>Activity Density / Human Presence</t>
+  </si>
+  <si>
+    <t>Crowd level, gatherings, events</t>
+  </si>
+  <si>
+    <t>Crowd chatter, applause, children, PA systems, doors, footsteps</t>
+  </si>
+  <si>
+    <t>PANNs / YAMNet</t>
+  </si>
+  <si>
+    <t>FSD50K</t>
+  </si>
+  <si>
+    <t>Infrastructure / Urban Markers</t>
+  </si>
+  <si>
+    <t>Developed vs. remote area</t>
+  </si>
+  <si>
+    <t>Sirens, construction, power generators, train crossings, electric hum</t>
+  </si>
+  <si>
+    <t>PANNs / EfficientAT</t>
+  </si>
+  <si>
+    <t>AudioSet, FSD50K</t>
+  </si>
+  <si>
+    <t>Communication Context</t>
+  </si>
+  <si>
+    <t>Indoor room, call center, outdoor field</t>
+  </si>
+  <si>
+    <t>Echo/reverb, HVAC, typing, mic clipping, wind buffeting</t>
+  </si>
+  <si>
+    <t>pyannote.audio + room impulse response estimate</t>
+  </si>
+  <si>
+    <t>Own data / RIR simulations</t>
+  </si>
+  <si>
+    <t>Weather / Environment</t>
+  </si>
+  <si>
+    <t>Conditions, correlation with METOC</t>
+  </si>
+  <si>
+    <t>Rain, thunder, wind gusts, dripping, birds</t>
+  </si>
+  <si>
+    <t>Risk / Hostile Indicators</t>
+  </si>
+  <si>
+    <t>Security or emergency events</t>
+  </si>
+  <si>
+    <t>Gunshots, explosions, glass break, screams</t>
+  </si>
+  <si>
+    <t>MIVIA, Zenodo gunshot datasets</t>
+  </si>
+  <si>
+    <t>Speech Presence / Language</t>
+  </si>
+  <si>
+    <t>Speech vs. noise balance, language used</t>
+  </si>
+  <si>
+    <t>Speech, language, prosody</t>
+  </si>
+  <si>
+    <t>Whisper / pyannote.audio</t>
+  </si>
+  <si>
+    <t>Common Voice, VoxPopuli</t>
+  </si>
+  <si>
+    <t>Emotional Tone / Stress</t>
+  </si>
+  <si>
+    <t>Calm, urgency, panic</t>
+  </si>
+  <si>
+    <t>Speech tempo, pitch variation, breathing, shouting</t>
+  </si>
+  <si>
+    <t>Whisper embeddings + emotion classifier</t>
+  </si>
+  <si>
+    <t>RAVDESS, CREMA-D</t>
+  </si>
+  <si>
+    <t>Temporal Pattern / Rhythm</t>
+  </si>
+  <si>
+    <t>Time of day, tempo of environment</t>
+  </si>
+  <si>
+    <t>Birds at dawn, night insects, reduced traffic, music tempo</t>
+  </si>
+  <si>
+    <t>PANNs + timestamp context</t>
+  </si>
+  <si>
+    <t>Own data</t>
+  </si>
+  <si>
+    <t>Platform Type</t>
+  </si>
+  <si>
+    <t>Recording source (bodycam, drone, phone)</t>
+  </si>
+  <si>
+    <t>Mic signature, wind noise pattern, compression artifacts</t>
+  </si>
+  <si>
+    <t>CLAP embedding similarity</t>
+  </si>
+  <si>
+    <t>Self-labeled data</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Car engine, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>drone buzz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, helicopter rotors, train brakes, footsteps, tire vs. track noise</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MIVIA, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GunshotDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, PANNs fine-tuned</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Urban, rural, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>indoor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, coastal, etc.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,13 +348,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,8 +413,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,11 +790,244 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9289F7A-1497-412B-82E3-1EE8F549AC67}">
+  <dimension ref="B2:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="1.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="8.796875" style="1"/>
+    <col min="13" max="13" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="16" customFormat="1">
+      <c r="B3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" s="13" customFormat="1">
+      <c r="B4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="7" customFormat="1">
+      <c r="B6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" s="7" customFormat="1">
+      <c r="B7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" s="13" customFormat="1">
+      <c r="B9" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" s="9" customFormat="1">
+      <c r="B10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" s="11" customFormat="1">
+      <c r="B11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" s="7" customFormat="1">
+      <c r="B13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1D2F39-08A9-4225-A59C-5EF116F1290C}">
-  <dimension ref="B3:E19"/>
+  <dimension ref="B3:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -472,27 +1038,27 @@
     <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -500,25 +1066,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:5">
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
       <c r="E12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="2:5">
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -526,12 +1101,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:9">
       <c r="B15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:9">
       <c r="B16" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
scenarios added 1 and 2 recorded
</commit_message>
<xml_diff>
--- a/resources/Brain Dump.xlsx
+++ b/resources/Brain Dump.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\echologia\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53A452CA-3E4F-43F8-A9D4-65F791286123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871079B0-C2E5-4453-B60D-C263EBE02452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C544BCDC-9C78-46B8-B4C5-15391AB69DE9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C544BCDC-9C78-46B8-B4C5-15391AB69DE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes for detection" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Scenario" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,67 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
-  <si>
-    <t>open source librayr</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Intent</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>People</t>
-  </si>
-  <si>
-    <t>Identitifcation</t>
-  </si>
-  <si>
-    <t>Wisper API</t>
-  </si>
-  <si>
-    <t>create a scenario</t>
-  </si>
-  <si>
-    <t>user display of the information</t>
-  </si>
-  <si>
-    <t>create raw data to inut</t>
-  </si>
-  <si>
-    <t>smoke break</t>
-  </si>
-  <si>
-    <t xml:space="preserve">have one MVP </t>
-  </si>
-  <si>
-    <t>conversation analyticcs</t>
-  </si>
-  <si>
-    <t>open source</t>
-  </si>
-  <si>
-    <t>Scales eazily</t>
-  </si>
-  <si>
-    <t>easy deploy</t>
-  </si>
-  <si>
-    <t>Recongnize</t>
-  </si>
-  <si>
-    <t>data basesfor raw data</t>
-  </si>
-  <si>
-    <t>list of files</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
   <si>
     <t>Attribute</t>
   </si>
@@ -335,12 +275,87 @@
       <t>, coastal, etc.</t>
     </r>
   </si>
+  <si>
+    <t>Audio 1</t>
+  </si>
+  <si>
+    <t>Church bell</t>
+  </si>
+  <si>
+    <t>Indoor</t>
+  </si>
+  <si>
+    <t>Outdoor</t>
+  </si>
+  <si>
+    <t>Gunshots</t>
+  </si>
+  <si>
+    <t>Audio 2</t>
+  </si>
+  <si>
+    <t>train crossing</t>
+  </si>
+  <si>
+    <t>helicopter</t>
+  </si>
+  <si>
+    <t>Audio 3</t>
+  </si>
+  <si>
+    <t>Audio 4</t>
+  </si>
+  <si>
+    <t>Audio 5</t>
+  </si>
+  <si>
+    <t>Audio 6</t>
+  </si>
+  <si>
+    <t>drone buzz</t>
+  </si>
+  <si>
+    <t>seawave</t>
+  </si>
+  <si>
+    <t>glass break</t>
+  </si>
+  <si>
+    <t>horns</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>construction site</t>
+  </si>
+  <si>
+    <t>screams</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Test Data file</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +386,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -415,7 +443,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -431,32 +458,33 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,227 +821,225 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9289F7A-1497-412B-82E3-1EE8F549AC67}">
   <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="1.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="8.796875" style="1"/>
-    <col min="13" max="13" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.796875" style="1"/>
+    <col min="1" max="1" width="1.796875" customWidth="1"/>
+    <col min="2" max="2" width="31.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.8984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="15" customFormat="1">
+      <c r="B3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" s="12" customFormat="1">
+      <c r="B4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="6" customFormat="1">
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="7" spans="2:6" s="6" customFormat="1">
+      <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" s="16" customFormat="1">
-      <c r="B3" s="14" t="s">
+      <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="15" t="s">
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" s="13" customFormat="1">
-      <c r="B4" s="17" t="s">
+      <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" s="12" customFormat="1">
+      <c r="B9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="3" t="s">
+      <c r="D9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="4" t="s">
+    </row>
+    <row r="10" spans="2:6" s="8" customFormat="1">
+      <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" s="7" customFormat="1">
-      <c r="B6" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="F10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="5" t="s">
+    </row>
+    <row r="11" spans="2:6" s="10" customFormat="1">
+      <c r="B11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="C11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="D11" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" s="7" customFormat="1">
-      <c r="B7" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="F11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="5" t="s">
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="4" t="s">
+    </row>
+    <row r="13" spans="2:6" s="6" customFormat="1">
+      <c r="B13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" s="13" customFormat="1">
-      <c r="B9" s="17" t="s">
+      <c r="C13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="E13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="F13" s="4" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" s="9" customFormat="1">
-      <c r="B10" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" s="11" customFormat="1">
-      <c r="B11" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" s="7" customFormat="1">
-      <c r="B13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1024,109 +1050,127 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1D2F39-08A9-4225-A59C-5EF116F1290C}">
-  <dimension ref="B3:I19"/>
+  <dimension ref="B4:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="25.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.09765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
+    <row r="4" spans="2:6">
+      <c r="B4" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9">
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>16</v>
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="F15" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>